<commit_message>
Update the PPD lab
It uses the front lines before start and after end lines, create a buffer of three lines that change progressively
</commit_message>
<xml_diff>
--- a/Year 3/Parallel and Distributed Programming/Laboratory 2/C++/Laboratory 2 C++.xlsx
+++ b/Year 3/Parallel and Distributed Programming/Laboratory 2/C++/Laboratory 2 C++.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\University\Year 3\Parallel and Distributed Programming\Laboratory 2\C++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9667D2EF-78BE-41E4-9A92-8A7F482921D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7BE43C-C43C-4C59-8824-7F4230E7ECD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,12 +110,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -293,40 +292,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>9.4800000000000006E-3</c:v>
+                  <c:v>1.018E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.38417000000000001</c:v>
+                  <c:v>0.44951000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>83.134659999999997</c:v>
+                  <c:v>89.825320000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.303759999999997</c:v>
+                  <c:v>15.90082</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.120950000000001</c:v>
+                  <c:v>8.5801599999999993</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.93338</c:v>
+                  <c:v>6.34335</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.586460000000001</c:v>
+                  <c:v>5.4871999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8419.4520100000009</c:v>
+                  <c:v>8908.5032300000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4226.9958699999997</c:v>
+                  <c:v>1538.4598800000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2374.90004</c:v>
+                  <c:v>776.24507000000006</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1462.8332700000001</c:v>
+                  <c:v>463.55248</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1267.606</c:v>
+                  <c:v>396.94342999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1373,7 +1372,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+      <selection activeCell="C2" sqref="C2:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,8 +1407,8 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2">
-        <v>9.4800000000000006E-3</v>
+      <c r="D2">
+        <v>1.018E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1418,8 +1417,8 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2">
-        <v>0.38417000000000001</v>
+      <c r="D3">
+        <v>0.44951000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1432,8 +1431,8 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2">
-        <v>83.134659999999997</v>
+      <c r="D4">
+        <v>89.825320000000005</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1442,8 +1441,8 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2">
-        <v>42.303759999999997</v>
+      <c r="D5">
+        <v>15.90082</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1452,8 +1451,8 @@
       <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2">
-        <v>23.120950000000001</v>
+      <c r="D6">
+        <v>8.5801599999999993</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1462,8 +1461,8 @@
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="2">
-        <v>12.93338</v>
+      <c r="D7">
+        <v>6.34335</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1472,8 +1471,8 @@
       <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="2">
-        <v>12.586460000000001</v>
+      <c r="D8">
+        <v>5.4871999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1486,8 +1485,8 @@
       <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="2">
-        <v>8419.4520100000009</v>
+      <c r="D9">
+        <v>8908.5032300000003</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1496,8 +1495,8 @@
       <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="2">
-        <v>4226.9958699999997</v>
+      <c r="D10">
+        <v>1538.4598800000001</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1506,8 +1505,8 @@
       <c r="C11" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="2">
-        <v>2374.90004</v>
+      <c r="D11">
+        <v>776.24507000000006</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1516,8 +1515,8 @@
       <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="2">
-        <v>1462.8332700000001</v>
+      <c r="D12">
+        <v>463.55248</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1526,8 +1525,8 @@
       <c r="C13" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="2">
-        <v>1267.606</v>
+      <c r="D13">
+        <v>396.94342999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>